<commit_message>
[Vedhashni] Added the file refactored code for end to end automation
</commit_message>
<xml_diff>
--- a/AmazonAssignment/DataForTesting/ExcelDataAmazon.xlsx
+++ b/AmazonAssignment/DataForTesting/ExcelDataAmazon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vedhashni.v\source\repos\AmazonAssignment\AmazonAssignment\DataForTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD70E0F-155C-4AEF-8F15-17F679258DEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6BF89E-00DC-4C2C-8B77-E27BEE391D11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{5F305000-E841-4BF4-99F8-1A75079E39F3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Email</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Vedha@1</t>
+  </si>
+  <si>
+    <t>vedhashni@1</t>
   </si>
 </sst>
 </file>
@@ -441,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC66A78-B5EF-4E90-879F-762E3721D55B}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,6 +526,14 @@
         <v>17</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{2E93158B-C57D-470D-9620-9659EC1EB9E7}"/>
@@ -530,6 +541,8 @@
     <hyperlink ref="E2" r:id="rId3" xr:uid="{37122512-44FB-4A46-8641-7941C9081ECC}"/>
     <hyperlink ref="I2" r:id="rId4" xr:uid="{0037C4E1-0120-4D71-BCE2-C7A5BDE48102}"/>
     <hyperlink ref="J2" r:id="rId5" xr:uid="{A64C0526-19CB-48A0-B69F-680C9A9AE606}"/>
+    <hyperlink ref="A3" r:id="rId6" xr:uid="{E7321DD6-7E8A-465B-87C3-83C34EC1A709}"/>
+    <hyperlink ref="B3" r:id="rId7" xr:uid="{024E7001-82AD-4ECD-BB6A-3C835B86E590}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>